<commit_message>
Sentence caser: NLP adjustments and bug squashing
</commit_message>
<xml_diff>
--- a/static/medical_societies.xlsx
+++ b/static/medical_societies.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chad\Dropbox\Data Box\Bella\test\Sentence Caser\word lists\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Chad\Dropbox\Data Box\Bella\zappa_app2\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBF8ADFA-1857-46D7-A033-DCE5810D5F3C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B60E4F-8516-4DBF-9719-2DA36543443C}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="20" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="595">
   <si>
     <t>name</t>
   </si>
@@ -1802,6 +1802,9 @@
   </si>
   <si>
     <t>Cochrane Collaboration</t>
+  </si>
+  <si>
+    <t>Food and Drug Administration</t>
   </si>
 </sst>
 </file>
@@ -2203,10 +2206,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A594"/>
+  <dimension ref="A1:A595"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A435" workbookViewId="0">
-      <selection activeCell="A440" sqref="A440:XFD440"/>
+    <sheetView tabSelected="1" topLeftCell="A378" workbookViewId="0">
+      <selection activeCell="A392" sqref="A392:XFD392"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4168,1016 +4171,1021 @@
     </row>
     <row r="392" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A392" t="s">
-        <v>389</v>
+        <v>594</v>
       </c>
     </row>
     <row r="393" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A393" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="394" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A394" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="395" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A395" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="396" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A396" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="397" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A397" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="398" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A398" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="399" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A399" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="400" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A400" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="401" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A401" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="402" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A402" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="403" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A403" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="404" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A404" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="405" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A405" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="406" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A406" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="407" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A407" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="408" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A408" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="409" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A409" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="410" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A410" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="411" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A411" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="412" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A412" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="413" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A413" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="414" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A414" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="415" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A415" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="416" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A416" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="417" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A417" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="418" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A418" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="419" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A419" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="420" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A420" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="421" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A421" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="422" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A422" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="423" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A423" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="424" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A424" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="425" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A425" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="426" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A426" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="427" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A427" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="428" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A428" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="429" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A429" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="430" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A430" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="431" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A431" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="432" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A432" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="433" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A433" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="434" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A434" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="435" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A435" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="436" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A436" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="437" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A437" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="438" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A438" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="439" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A439" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
     </row>
     <row r="440" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A440" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
     </row>
     <row r="441" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A441" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
     </row>
     <row r="442" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A442" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="443" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A443" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="444" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A444" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="445" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A445" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="446" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A446" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="447" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A447" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="448" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A448" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="449" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A449" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="450" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A450" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
     </row>
     <row r="451" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A451" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="452" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A452" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
     </row>
     <row r="453" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A453" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="454" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A454" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="455" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A455" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="456" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A456" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="457" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A457" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
     </row>
     <row r="458" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A458" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
     </row>
     <row r="459" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A459" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="460" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A460" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="461" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A461" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="462" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A462" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="463" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A463" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="464" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A464" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="465" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A465" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="466" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A466" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="467" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A467" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="468" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A468" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="469" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A469" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="470" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A470" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="471" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A471" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="472" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A472" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="473" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A473" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
     </row>
     <row r="474" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A474" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="475" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A475" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="476" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A476" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="477" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A477" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="478" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A478" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="479" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A479" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
     </row>
     <row r="480" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A480" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="481" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A481" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
     </row>
     <row r="482" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A482" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
     </row>
     <row r="483" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A483" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
     </row>
     <row r="484" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A484" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
     </row>
     <row r="485" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A485" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="486" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A486" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
     </row>
     <row r="487" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A487" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="488" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A488" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="489" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A489" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
     </row>
     <row r="490" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A490" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="491" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A491" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="492" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A492" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="493" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A493" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="494" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A494" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="495" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A495" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="496" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A496" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="497" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A497" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="498" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A498" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="499" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A499" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
     </row>
     <row r="500" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A500" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="501" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A501" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="502" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A502" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="503" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A503" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="504" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A504" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="505" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A505" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
     </row>
     <row r="506" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A506" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="507" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A507" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="508" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A508" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="509" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A509" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="510" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A510" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="511" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A511" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="512" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A512" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="513" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A513" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="514" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A514" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="515" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A515" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="516" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A516" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
     </row>
     <row r="517" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A517" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="518" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A518" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
     </row>
     <row r="519" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A519" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
     </row>
     <row r="520" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A520" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="521" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A521" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
     </row>
     <row r="522" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A522" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="523" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A523" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
     </row>
     <row r="524" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A524" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
     </row>
     <row r="525" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A525" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="526" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A526" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="527" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A527" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="528" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A528" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="529" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A529" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="530" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A530" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="531" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A531" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="532" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A532" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="533" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A533" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="534" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A534" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="535" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A535" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="536" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A536" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="537" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A537" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="538" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A538" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="539" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A539" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="540" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A540" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="541" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A541" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="542" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A542" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="543" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A543" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="544" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A544" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="545" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A545" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="546" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A546" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="547" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A547" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="548" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A548" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="549" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A549" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="550" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A550" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="551" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A551" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="552" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A552" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="553" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A553" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="554" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A554" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="555" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A555" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="556" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A556" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="557" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A557" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="558" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A558" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="559" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A559" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="560" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A560" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="561" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A561" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="562" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A562" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="563" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A563" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="564" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A564" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="565" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A565" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="566" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A566" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="567" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A567" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="568" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A568" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="569" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A569" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="570" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A570" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="571" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A571" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="572" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A572" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="573" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A573" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="574" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A574" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="575" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A575" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="576" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A576" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="577" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A577" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="578" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A578" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="579" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A579" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="580" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A580" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="581" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A581" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="582" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A582" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="583" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A583" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="584" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A584" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="585" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A585" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="586" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A586" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="587" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A587" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="588" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A588" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="589" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A589" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="590" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A590" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="591" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A591" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="592" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A592" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="593" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A593" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="594" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A594" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="595" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A595" t="s">
         <v>591</v>
       </c>
     </row>

</xml_diff>